<commit_message>
Sujit - updated excel with quartely field.
</commit_message>
<xml_diff>
--- a/GST LIST 25 Oct 2023 (Autosaved).xlsx
+++ b/GST LIST 25 Oct 2023 (Autosaved).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujit jha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BusyGirRepo\busydata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="640">
   <si>
     <t>SRl No.</t>
   </si>
@@ -2672,6 +2672,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2699,7 +2700,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3286,10 +3286,10 @@
   <dimension ref="A1:W91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R31" sqref="R31"/>
+      <selection pane="bottomRight" activeCell="A63" sqref="A63:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,11 +3321,11 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="117"/>
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="140" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="118"/>
       <c r="F1" s="118"/>
       <c r="G1" s="118"/>
@@ -6244,6 +6244,9 @@
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="B65" s="7">
         <v>64</v>
       </c>
@@ -6264,6 +6267,9 @@
       </c>
     </row>
     <row r="66" spans="1:23" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>367</v>
+      </c>
       <c r="B66" s="74">
         <v>65</v>
       </c>
@@ -6287,6 +6293,9 @@
       <c r="W66" s="75"/>
     </row>
     <row r="67" spans="1:23" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="B67" s="74">
         <v>66</v>
       </c>
@@ -6310,6 +6319,9 @@
       <c r="W67" s="75"/>
     </row>
     <row r="68" spans="1:23" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>367</v>
+      </c>
       <c r="B68" s="74">
         <v>67</v>
       </c>
@@ -6330,6 +6342,9 @@
       <c r="W68" s="75"/>
     </row>
     <row r="69" spans="1:23" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="B69" s="74">
         <v>68</v>
       </c>
@@ -6409,7 +6424,7 @@
         <v>638</v>
       </c>
       <c r="D72" s="7"/>
-      <c r="E72" s="148" t="s">
+      <c r="E72" s="139" t="s">
         <v>639</v>
       </c>
       <c r="F72" s="79"/>
@@ -6948,10 +6963,10 @@
       </c>
     </row>
     <row r="8" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F8" s="145" t="s">
+      <c r="F8" s="146" t="s">
         <v>299</v>
       </c>
-      <c r="G8" s="146"/>
+      <c r="G8" s="147"/>
       <c r="M8" t="s">
         <v>593</v>
       </c>
@@ -8230,10 +8245,10 @@
         <f>SUM(D3:D81)</f>
         <v>50131</v>
       </c>
-      <c r="H2" s="147" t="s">
+      <c r="H2" s="148" t="s">
         <v>583</v>
       </c>
-      <c r="I2" s="147"/>
+      <c r="I2" s="148"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -9246,15 +9261,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -9478,16 +9493,16 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="143" t="s">
+      <c r="B13" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -9701,16 +9716,16 @@
       <c r="F21" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="141" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="142"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="143"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -11445,44 +11460,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C1" s="144" t="s">
+      <c r="C1" s="145" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
     </row>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="144"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="145"/>
     </row>
     <row r="3" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C3" s="140" t="s">
+      <c r="C3" s="141" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -11798,18 +11813,18 @@
       <c r="L13" s="1"/>
     </row>
     <row r="15" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C15" s="140" t="s">
+      <c r="C15" s="141" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="141"/>
-      <c r="G15" s="141"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="141"/>
-      <c r="J15" s="141"/>
-      <c r="K15" s="141"/>
-      <c r="L15" s="142"/>
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="142"/>
+      <c r="L15" s="143"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
@@ -12125,18 +12140,18 @@
       <c r="L25" s="1"/>
     </row>
     <row r="28" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C28" s="140" t="s">
+      <c r="C28" s="141" t="s">
         <v>210</v>
       </c>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="141"/>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="141"/>
-      <c r="L28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="142"/>
+      <c r="K28" s="142"/>
+      <c r="L28" s="143"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
@@ -12225,18 +12240,18 @@
       <c r="L31" s="1"/>
     </row>
     <row r="34" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C34" s="140" t="s">
+      <c r="C34" s="141" t="s">
         <v>211</v>
       </c>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="141"/>
-      <c r="G34" s="141"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="141"/>
-      <c r="J34" s="141"/>
-      <c r="K34" s="141"/>
-      <c r="L34" s="142"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="142"/>
+      <c r="I34" s="142"/>
+      <c r="J34" s="142"/>
+      <c r="K34" s="142"/>
+      <c r="L34" s="143"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
@@ -12552,18 +12567,18 @@
       <c r="L44" s="1"/>
     </row>
     <row r="47" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C47" s="140" t="s">
+      <c r="C47" s="141" t="s">
         <v>212</v>
       </c>
-      <c r="D47" s="141"/>
-      <c r="E47" s="141"/>
-      <c r="F47" s="141"/>
-      <c r="G47" s="141"/>
-      <c r="H47" s="141"/>
-      <c r="I47" s="141"/>
-      <c r="J47" s="141"/>
-      <c r="K47" s="141"/>
-      <c r="L47" s="142"/>
+      <c r="D47" s="142"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="142"/>
+      <c r="G47" s="142"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="142"/>
+      <c r="J47" s="142"/>
+      <c r="K47" s="142"/>
+      <c r="L47" s="143"/>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -12652,18 +12667,18 @@
       <c r="L50" s="1"/>
     </row>
     <row r="53" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C53" s="140" t="s">
+      <c r="C53" s="141" t="s">
         <v>213</v>
       </c>
-      <c r="D53" s="141"/>
-      <c r="E53" s="141"/>
-      <c r="F53" s="141"/>
-      <c r="G53" s="141"/>
-      <c r="H53" s="141"/>
-      <c r="I53" s="141"/>
-      <c r="J53" s="141"/>
-      <c r="K53" s="141"/>
-      <c r="L53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="142"/>
+      <c r="F53" s="142"/>
+      <c r="G53" s="142"/>
+      <c r="H53" s="142"/>
+      <c r="I53" s="142"/>
+      <c r="J53" s="142"/>
+      <c r="K53" s="142"/>
+      <c r="L53" s="143"/>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -12752,18 +12767,18 @@
       <c r="L56" s="1"/>
     </row>
     <row r="60" spans="3:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C60" s="140" t="s">
+      <c r="C60" s="141" t="s">
         <v>214</v>
       </c>
-      <c r="D60" s="141"/>
-      <c r="E60" s="141"/>
-      <c r="F60" s="141"/>
-      <c r="G60" s="141"/>
-      <c r="H60" s="141"/>
-      <c r="I60" s="141"/>
-      <c r="J60" s="141"/>
-      <c r="K60" s="141"/>
-      <c r="L60" s="142"/>
+      <c r="D60" s="142"/>
+      <c r="E60" s="142"/>
+      <c r="F60" s="142"/>
+      <c r="G60" s="142"/>
+      <c r="H60" s="142"/>
+      <c r="I60" s="142"/>
+      <c r="J60" s="142"/>
+      <c r="K60" s="142"/>
+      <c r="L60" s="143"/>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">

</xml_diff>